<commit_message>
ResultEntry and work received updated
</commit_message>
<xml_diff>
--- a/src/main/resources/Lab Episodes Registrations.xlsx
+++ b/src/main/resources/Lab Episodes Registrations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TrakCareTesting\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D948458-ECD1-4D60-A706-20B601B550D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252DFD18-C19D-4006-ABCD-5CE882F0FAB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3468" yWindow="2844" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="6" xr2:uid="{A9080B75-4E5F-4478-AAE2-7149856FF9B4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A9080B75-4E5F-4478-AAE2-7149856FF9B4}"/>
   </bookViews>
   <sheets>
     <sheet name="PatientInfo" sheetId="3" r:id="rId1"/>
@@ -842,7 +842,7 @@
     <t>AliquotTest Set</t>
   </si>
   <si>
-    <t>PatientKey</t>
+    <t>PatientKey_FK</t>
   </si>
 </sst>
 </file>
@@ -1313,7 +1313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4AF9EB-04F9-4C5F-83CD-5EC797FC584F}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -2850,8 +2850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4BD0E40-ADE9-4A1F-8FCD-B7AD0D5A0136}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2979,6 +2979,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Lastupdated xmlns="36f692a8-3d33-41c6-9b2b-598d6edaefd0" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="36f692a8-3d33-41c6-9b2b-598d6edaefd0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d2a6fb75-4833-4c65-a592-c6a2bce7c31e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003EAF60C23A9AF146B878708D06FCA971" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c90c546dab3258d1dee7c6a81b5cbd18">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="36f692a8-3d33-41c6-9b2b-598d6edaefd0" xmlns:ns3="d2a6fb75-4833-4c65-a592-c6a2bce7c31e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f16b141dceb693e0600ffa6c7add9171" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3232,30 +3255,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Lastupdated xmlns="36f692a8-3d33-41c6-9b2b-598d6edaefd0" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="36f692a8-3d33-41c6-9b2b-598d6edaefd0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d2a6fb75-4833-4c65-a592-c6a2bce7c31e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{315D34F6-D5ED-4574-B268-05744C736FC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD04A7C0-83A7-4DED-B6EA-7CF1A8E604F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="36f692a8-3d33-41c6-9b2b-598d6edaefd0"/>
+    <ds:schemaRef ds:uri="d2a6fb75-4833-4c65-a592-c6a2bce7c31e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6F20231-C530-4980-8436-61646849E7DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3273,24 +3293,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD04A7C0-83A7-4DED-B6EA-7CF1A8E604F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="36f692a8-3d33-41c6-9b2b-598d6edaefd0"/>
-    <ds:schemaRef ds:uri="d2a6fb75-4833-4c65-a592-c6a2bce7c31e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{315D34F6-D5ED-4574-B268-05744C736FC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>